<commit_message>
feat(xlsx): write xlsx by reflect
</commit_message>
<xml_diff>
--- a/utils/xlsx/test_write.xlsx
+++ b/utils/xlsx/test_write.xlsx
@@ -330,15 +330,23 @@
         <v>姓名</v>
       </c>
       <c r="B1" t="str">
-        <v>年龄</v>
+        <v>年齡</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>狗子</v>
+        <v>小明</v>
       </c>
       <c r="B2" t="str">
-        <v>18</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>小华</v>
+      </c>
+      <c r="B3" t="str">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(xlsx): fix the xlsx write type
</commit_message>
<xml_diff>
--- a/utils/xlsx/test_write.xlsx
+++ b/utils/xlsx/test_write.xlsx
@@ -337,7 +337,7 @@
       <c r="A2" t="str">
         <v>小明</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2">
         <v>11</v>
       </c>
     </row>
@@ -345,7 +345,7 @@
       <c r="A3" t="str">
         <v>小华</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3">
         <v>12</v>
       </c>
     </row>

</xml_diff>